<commit_message>
Modification template "Etat de réception des emballages plastique" Ajout n° contrat stat Tonnage répartition
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/EtatMensuelReception.xlsx
+++ b/eVaSys.Server/Assets/Templates/EtatMensuelReception.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Repos\Valorplast\eValorplastWebApp\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B44BAA-9CF8-4778-A607-F63214DE468F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D21AA1D-DBFF-4513-9043-55D5847CA56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12648" yWindow="4200" windowWidth="23364" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6144" yWindow="6144" windowWidth="15540" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etat" sheetId="4" r:id="rId1"/>
     <sheet name="Répartition" sheetId="3" r:id="rId2"/>
     <sheet name="Produits" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -96,7 +96,7 @@
     <t xml:space="preserve">Paris le </t>
   </si>
   <si>
-    <t>L'état des réceptions des emballages plastique est établi sur la base des déclarations que vous avez faites à Valorplast. Il indique la répartition des tonnages entre les différents contrats que vous gérez. Cet état ne peut en aucun cas servir de justificatif auprès de CITEO ou d'Adelphe pour tout règlement.</t>
+    <t>L'état des réceptions des emballages plastique est établi sur la base des déclarations que vous avez faites à Valorplast. Il indique la répartition des tonnages entre les différents contrats que vous gérez. Cet état ne peut en aucun cas servir de justificatif auprès des éco-organismes pour tout règlement.</t>
   </si>
 </sst>
 </file>
@@ -337,13 +337,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -8002,11 +8002,11 @@
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="8" t="s">
         <v>16</v>
       </c>
@@ -8015,606 +8015,686 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="6"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="6"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
       <c r="E57" s="6"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="6"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
       <c r="E59" s="6"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="6"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
       <c r="E62" s="6"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
       <c r="E64" s="6"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="6"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="6"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
       <c r="E68" s="6"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="6"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="6"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="6"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
       <c r="E72" s="6"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="6"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
       <c r="E74" s="6"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="28"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="6"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="28"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
       <c r="E76" s="6"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="28"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
       <c r="E77" s="6"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="28"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
       <c r="E78" s="6"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="28"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="6"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="28"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
       <c r="E80" s="6"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="6"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="28"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="6"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="6"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
       <c r="E84" s="6"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="6"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30"/>
       <c r="E86" s="6"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
       <c r="E87" s="6"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="28"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="6"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="28"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="28"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
       <c r="E89" s="6"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="28"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30"/>
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="6"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
       <c r="E94" s="6"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="30"/>
       <c r="E95" s="6"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30"/>
       <c r="E96" s="6"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
       <c r="E98" s="6"/>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="28"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
       <c r="E99" s="6"/>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
       <c r="E100" s="6"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
+      <c r="B101" s="30"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="30"/>
       <c r="E101" s="6"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
+      <c r="B102" s="30"/>
+      <c r="C102" s="30"/>
+      <c r="D102" s="30"/>
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="28"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
+      <c r="B103" s="30"/>
+      <c r="C103" s="30"/>
+      <c r="D103" s="30"/>
       <c r="E103" s="6"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="28"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
+      <c r="B104" s="30"/>
+      <c r="C104" s="30"/>
+      <c r="D104" s="30"/>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="28"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
+      <c r="B105" s="30"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="30"/>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="28"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
+      <c r="B106" s="30"/>
+      <c r="C106" s="30"/>
+      <c r="D106" s="30"/>
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
       <c r="E107" s="6"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="28"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
+      <c r="B108" s="30"/>
+      <c r="C108" s="30"/>
+      <c r="D108" s="30"/>
       <c r="E108" s="6"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="28"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
+      <c r="B109" s="30"/>
+      <c r="C109" s="30"/>
+      <c r="D109" s="30"/>
       <c r="E109" s="6"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
       <c r="E110" s="6"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="28"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
+      <c r="B111" s="30"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
       <c r="E111" s="6"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
       <c r="E112" s="6"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="30"/>
       <c r="E113" s="6"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="28"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
+      <c r="B114" s="30"/>
+      <c r="C114" s="30"/>
+      <c r="D114" s="30"/>
       <c r="E114" s="6"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="28"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="28"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="30"/>
+      <c r="D115" s="30"/>
       <c r="E115" s="6"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
+      <c r="B116" s="30"/>
+      <c r="C116" s="30"/>
+      <c r="D116" s="30"/>
       <c r="E116" s="6"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="28"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="30"/>
+      <c r="D117" s="30"/>
       <c r="E117" s="6"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="28"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="28"/>
+      <c r="B118" s="30"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
       <c r="E118" s="6"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="28"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="28"/>
+      <c r="B119" s="30"/>
+      <c r="C119" s="30"/>
+      <c r="D119" s="30"/>
       <c r="E119" s="6"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="28"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="30"/>
+      <c r="D120" s="30"/>
       <c r="E120" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B120:D120"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -8625,91 +8705,11 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B120:D120"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>